<commit_message>
Added some info about Supporting tools
</commit_message>
<xml_diff>
--- a/302 Role information.xlsx
+++ b/302 Role information.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarod/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarod/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4953CD1E-96BA-B544-A568-6187C4A12A75}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDDB3E9-EAAE-3546-BC08-D57CDF51AEE3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="0" windowWidth="14200" windowHeight="18000" xr2:uid="{EC68C681-57E9-8E48-95CA-F0633512305D}"/>
+    <workbookView xWindow="14600" yWindow="460" windowWidth="14200" windowHeight="17540" xr2:uid="{EC68C681-57E9-8E48-95CA-F0633512305D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">Admin </t>
   </si>
@@ -58,6 +58,45 @@
   </si>
   <si>
     <t>Salary / Year</t>
+  </si>
+  <si>
+    <t>Supporting tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visualization </t>
+  </si>
+  <si>
+    <t>ERP</t>
+  </si>
+  <si>
+    <t>Reporting &amp; Analysis system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Production Planning &amp; Control system </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Machine execution systems </t>
+  </si>
+  <si>
+    <t>Internet of Users &amp; Internet of thigns</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>BUDGET</t>
+  </si>
+  <si>
+    <t>https://blog.clientsfirst-tx.com/blog-1/how-much-is-erp</t>
+  </si>
+  <si>
+    <t>https://www.zoho.com/analytics/pricing.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>How Many</t>
   </si>
 </sst>
 </file>
@@ -67,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +126,14 @@
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,17 +152,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,20 +478,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A846233-7B51-8948-B796-690427504E13}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="33" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" customWidth="1"/>
     <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24">
+    <row r="1" spans="1:5" ht="24">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -451,8 +502,14 @@
       <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -463,8 +520,14 @@
       <c r="C2" s="3">
         <v>150000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>750000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -476,7 +539,7 @@
         <v>123000</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -488,7 +551,7 @@
         <v>102336</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -500,7 +563,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -512,7 +575,7 @@
         <v>91597</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -524,7 +587,7 @@
         <v>44491</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -536,7 +599,7 @@
         <v>66080</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -548,7 +611,67 @@
         <v>54017</v>
       </c>
     </row>
+    <row r="13" spans="1:5" ht="24">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4">
+        <v>125000</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1186</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>19200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C15" r:id="rId1" xr:uid="{711F9200-36C2-2545-BF2B-DE8B93898DCE}"/>
+    <hyperlink ref="C16" r:id="rId2" xr:uid="{9641BF4E-5B3D-674E-8AF7-CE890F987B28}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>